<commit_message>
feat : adding smoke and Fire to the rocket
</commit_message>
<xml_diff>
--- a/documentation/planning/StellaStone - Planning - S1.xlsx
+++ b/documentation/planning/StellaStone - Planning - S1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20140FD0-1D72-4803-B9F2-E825E37001EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB4B08C-47F4-45BF-BA49-3E50E2C71E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,9 +19,9 @@
     <definedName name="fin_tâche" localSheetId="0">PlanningProjet!$F1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">PlanningProjet!$4:$6</definedName>
     <definedName name="Semaine_Affichage">PlanningProjet!$E$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">PlanningProjet!$A$1:$BS$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PlanningProjet!$A$1:$BT$32</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,9 +29,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Créez un planning de projet dans cette feuille de calcul.
 Entrez le titre de ce projet dans la cellule B1. 
@@ -47,13 +50,7 @@
 Continuez à parcourir la colonne A pour entendre des instructions supplémentaires.</t>
   </si>
   <si>
-    <t>StellaStone</t>
-  </si>
-  <si>
     <t>Entrez le nom de la société dans la cellule B2.</t>
-  </si>
-  <si>
-    <t>Novus</t>
   </si>
   <si>
     <t>Entrez le nom du chef de projet dans la cellule B3. Entrez la date de début du projet dans la cellule E3. Début du projet : l’étiquette figure dans la cellule C3.</t>
@@ -109,9 +106,6 @@
 Pour supprimer la phase et travailler uniquement à partir de tâches, supprimez simplement cette ligne.</t>
   </si>
   <si>
-    <t>Phase 1 : Spécification des exigences format IEEE 830-1998</t>
-  </si>
-  <si>
     <t xml:space="preserve">La cellule B9 contient l’exemple de tâche « Tâche 1 ». 
 Entrez un nouveau nom de tâche dans la cellule B9.
 Entrez une personne à laquelle attribuer la tâche dans la cellule C9.
@@ -119,12 +113,6 @@
 Entrez la date de début de la tâche dans la cellule E9.
 Entrez la date de fin de tâche dans la cellule F9.
 Une barre d’état ombrée pour les dates entrées apparaît dans les blocs de la cellule I9 à la cellule BL9. </t>
-  </si>
-  <si>
-    <t>Benguezzou, Meziane, Rouabah, Zeghdallou</t>
-  </si>
-  <si>
-    <t>Phase 1.1 : Tests de recette</t>
   </si>
   <si>
     <t>La cellule à droite contient l’exemple titre Phase 2. 
@@ -137,44 +125,14 @@
 Répétez les instructions des cellules A8 et A9 chaque fois que c’est nécessaire.</t>
   </si>
   <si>
-    <t>Phase 2 : Conception générale format IEEE 1016-2009</t>
-  </si>
-  <si>
-    <t>Benguezzou, Meziane</t>
-  </si>
-  <si>
     <t>Exemple de bloc de titre de phase</t>
-  </si>
-  <si>
-    <t>Phase 3 : Tests d'intégration</t>
-  </si>
-  <si>
-    <t>Rouabah, Zaghdellou</t>
-  </si>
-  <si>
-    <t>Phase 3.1 : Manuel utilisateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phase 3.2 : Conception d'une maquette </t>
   </si>
   <si>
     <t>Ceci est une ligne vide.</t>
   </si>
   <si>
-    <t>Phase 4 : Relecture des documents par d'autre entreprise</t>
-  </si>
-  <si>
     <t>Cette ligne marque la fin du planning de projet. N’ENTREZ rien dans cette ligne. 
 Insérez de nouvelles lignes au-dessus de celle-ci pour continuer d’élaborer votre planning de projet.</t>
-  </si>
-  <si>
-    <t>Phase 4.1 : Finalisation et rectification des possibles erreurs</t>
-  </si>
-  <si>
-    <t>Phase 5 : Préparation de la soutenance</t>
-  </si>
-  <si>
-    <t>Phase 6 : Présentation de StellaStone</t>
   </si>
   <si>
     <t>DIAGRAMME DE GANTT SIMPLE par Vertex42.com</t>
@@ -225,6 +183,51 @@
   </si>
   <si>
     <t>Les entreprises trouveront également des modèles de facture, de feuille de temps, de suivi d’inventaire, d’états financiers et de planification de projet. Les enseignants et les étudiants pourront utiliser des ressources variées, notamment des emplois du temps, des carnets de notes et des feuilles de présence. Organisez votre vie famille avec des planificateurs de repas, des listes de contrôle et des journaux d’entraînement. Chaque modèle est minutieusement étudié, affiné et amélioré au fil du temps grâce aux commentaires de milliers d’utilisateurs.</t>
+  </si>
+  <si>
+    <t>Phase 1 : Choix du sujet et répartition des tâches</t>
+  </si>
+  <si>
+    <t>Meziane, Bouabid, Bougassaa, Benguezzou</t>
+  </si>
+  <si>
+    <t>Phase 1.1 : Planification</t>
+  </si>
+  <si>
+    <t>Phase 2 : Répartition des tâches et planning du reste</t>
+  </si>
+  <si>
+    <t>Phase 2.1 : Réalisation du document d'initialisation</t>
+  </si>
+  <si>
+    <t>Phase 2.2 : Réalisation du document de définition de l'application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phase 3 : Dévelopement </t>
+  </si>
+  <si>
+    <t>Phase 3.1 : Création de l'instance Wikibase et de l'interface d'exploitation</t>
+  </si>
+  <si>
+    <t>Phase 3.2 : Création des entités fondamentales et de l'interface utilisateur</t>
+  </si>
+  <si>
+    <t>Phase 4 : Extraction et ingestion des données sur Wikibase</t>
+  </si>
+  <si>
+    <t>25/02/2023</t>
+  </si>
+  <si>
+    <t>Phase 5 : Test de l'interaction utilisateur</t>
+  </si>
+  <si>
+    <t>Phase 5.1 : Test d'intégration</t>
+  </si>
+  <si>
+    <t>Phase 6 : Soutenance</t>
+  </si>
+  <si>
+    <t>Diagramme de Gantt</t>
   </si>
 </sst>
 </file>
@@ -498,7 +501,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="52">
+  <fills count="54">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -792,6 +795,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -1102,7 +1117,7 @@
     <xf numFmtId="0" fontId="7" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1258,9 +1273,6 @@
     <xf numFmtId="0" fontId="34" fillId="44" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="45" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="45" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1279,18 +1291,12 @@
     <xf numFmtId="0" fontId="34" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="47" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="5" fillId="48" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="48" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="48" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1330,14 +1336,50 @@
     <xf numFmtId="167" fontId="7" fillId="51" borderId="2" xfId="10" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="49" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="48" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="49" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="45" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="49" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="49" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
+    <xf numFmtId="0" fontId="34" fillId="52" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="52" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="52" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="52" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="52" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="53" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="53" borderId="2" xfId="10" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1348,6 +1390,18 @@
     <xf numFmtId="168" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="53" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="53" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="51" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
@@ -1355,43 +1409,31 @@
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="8" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="46" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="46" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="11" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="46" borderId="2" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="46" borderId="2" xfId="12" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1450,7 +1492,187 @@
     <cellStyle name="Vérification" xfId="25" builtinId="23" customBuiltin="1"/>
     <cellStyle name="zTexteMasqué" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="41">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1691,15 +1913,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ListeTâches" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="22"/>
-      <tableStyleElement type="headerRow" dxfId="21"/>
-      <tableStyleElement type="totalRow" dxfId="20"/>
-      <tableStyleElement type="firstColumn" dxfId="19"/>
-      <tableStyleElement type="lastColumn" dxfId="18"/>
-      <tableStyleElement type="firstRowStripe" dxfId="17"/>
-      <tableStyleElement type="secondRowStripe" dxfId="16"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="15"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="14"/>
+      <tableStyleElement type="wholeTable" dxfId="40"/>
+      <tableStyleElement type="headerRow" dxfId="39"/>
+      <tableStyleElement type="totalRow" dxfId="38"/>
+      <tableStyleElement type="firstColumn" dxfId="37"/>
+      <tableStyleElement type="lastColumn" dxfId="36"/>
+      <tableStyleElement type="firstRowStripe" dxfId="35"/>
+      <tableStyleElement type="secondRowStripe" dxfId="34"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="33"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="32"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2115,11 +2337,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BS28"/>
+  <dimension ref="A1:BS32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2147,7 +2369,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -2158,132 +2380,130 @@
     </row>
     <row r="2" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B2" s="33"/>
       <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="97"/>
-      <c r="E3" s="99">
-        <v>44851</v>
-      </c>
-      <c r="F3" s="99"/>
+      <c r="C3" s="91" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="92"/>
+      <c r="E3" s="97">
+        <v>44959</v>
+      </c>
+      <c r="F3" s="97"/>
     </row>
     <row r="4" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="96" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="97"/>
+        <v>4</v>
+      </c>
+      <c r="C4" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="92"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="84">
+      <c r="I4" s="93">
         <f>I5</f>
-        <v>44851</v>
-      </c>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="84">
+        <v>44956</v>
+      </c>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="93">
         <f>P5</f>
-        <v>44858</v>
-      </c>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="85"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="84">
+        <v>44963</v>
+      </c>
+      <c r="Q4" s="94"/>
+      <c r="R4" s="94"/>
+      <c r="S4" s="94"/>
+      <c r="T4" s="94"/>
+      <c r="U4" s="94"/>
+      <c r="V4" s="95"/>
+      <c r="W4" s="93">
         <f>W5</f>
-        <v>44865</v>
-      </c>
-      <c r="X4" s="85"/>
-      <c r="Y4" s="85"/>
-      <c r="Z4" s="85"/>
-      <c r="AA4" s="85"/>
-      <c r="AB4" s="85"/>
-      <c r="AC4" s="86"/>
-      <c r="AD4" s="84">
+        <v>44970</v>
+      </c>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="95"/>
+      <c r="AD4" s="93">
         <f>AD5</f>
-        <v>44872</v>
-      </c>
-      <c r="AE4" s="85"/>
-      <c r="AF4" s="85"/>
-      <c r="AG4" s="85"/>
-      <c r="AH4" s="85"/>
-      <c r="AI4" s="85"/>
-      <c r="AJ4" s="86"/>
-      <c r="AK4" s="84">
+        <v>44977</v>
+      </c>
+      <c r="AE4" s="94"/>
+      <c r="AF4" s="94"/>
+      <c r="AG4" s="94"/>
+      <c r="AH4" s="94"/>
+      <c r="AI4" s="94"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="93">
         <f>AK5</f>
-        <v>44879</v>
-      </c>
-      <c r="AL4" s="85"/>
-      <c r="AM4" s="85"/>
-      <c r="AN4" s="85"/>
-      <c r="AO4" s="85"/>
-      <c r="AP4" s="85"/>
-      <c r="AQ4" s="86"/>
-      <c r="AR4" s="84">
+        <v>44984</v>
+      </c>
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
+      <c r="AN4" s="94"/>
+      <c r="AO4" s="94"/>
+      <c r="AP4" s="94"/>
+      <c r="AQ4" s="95"/>
+      <c r="AR4" s="93">
         <f>AR5</f>
-        <v>44886</v>
-      </c>
-      <c r="AS4" s="85"/>
-      <c r="AT4" s="85"/>
-      <c r="AU4" s="85"/>
-      <c r="AV4" s="85"/>
-      <c r="AW4" s="85"/>
-      <c r="AX4" s="86"/>
-      <c r="AY4" s="84">
+        <v>44991</v>
+      </c>
+      <c r="AS4" s="94"/>
+      <c r="AT4" s="94"/>
+      <c r="AU4" s="94"/>
+      <c r="AV4" s="94"/>
+      <c r="AW4" s="94"/>
+      <c r="AX4" s="95"/>
+      <c r="AY4" s="93">
         <f>AY5</f>
-        <v>44893</v>
-      </c>
-      <c r="AZ4" s="85"/>
-      <c r="BA4" s="85"/>
-      <c r="BB4" s="85"/>
-      <c r="BC4" s="85"/>
-      <c r="BD4" s="85"/>
-      <c r="BE4" s="86"/>
-      <c r="BF4" s="84">
+        <v>44998</v>
+      </c>
+      <c r="AZ4" s="94"/>
+      <c r="BA4" s="94"/>
+      <c r="BB4" s="94"/>
+      <c r="BC4" s="94"/>
+      <c r="BD4" s="94"/>
+      <c r="BE4" s="95"/>
+      <c r="BF4" s="93">
         <f>BF5</f>
-        <v>44900</v>
-      </c>
-      <c r="BG4" s="85"/>
-      <c r="BH4" s="85"/>
-      <c r="BI4" s="85"/>
-      <c r="BJ4" s="85"/>
-      <c r="BK4" s="85"/>
-      <c r="BL4" s="86"/>
-      <c r="BM4" s="84">
+        <v>45005</v>
+      </c>
+      <c r="BG4" s="94"/>
+      <c r="BH4" s="94"/>
+      <c r="BI4" s="94"/>
+      <c r="BJ4" s="94"/>
+      <c r="BK4" s="94"/>
+      <c r="BL4" s="95"/>
+      <c r="BM4" s="93">
         <f>BM5</f>
-        <v>44907</v>
-      </c>
-      <c r="BN4" s="85"/>
-      <c r="BO4" s="85"/>
-      <c r="BP4" s="85"/>
-      <c r="BQ4" s="85"/>
-      <c r="BR4" s="85"/>
-      <c r="BS4" s="86"/>
+        <v>45012</v>
+      </c>
+      <c r="BN4" s="94"/>
+      <c r="BO4" s="94"/>
+      <c r="BP4" s="94"/>
+      <c r="BQ4" s="94"/>
+      <c r="BR4" s="94"/>
+      <c r="BS4" s="95"/>
     </row>
     <row r="5" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
@@ -2293,277 +2513,277 @@
       <c r="G5" s="38"/>
       <c r="I5" s="51">
         <f>Début_Projet-WEEKDAY(Début_Projet,1)+2+7*(Semaine_Affichage-1)</f>
-        <v>44851</v>
+        <v>44956</v>
       </c>
       <c r="J5" s="52">
         <f>I5+1</f>
-        <v>44852</v>
+        <v>44957</v>
       </c>
       <c r="K5" s="52">
         <f t="shared" ref="K5:AX5" si="0">J5+1</f>
-        <v>44853</v>
+        <v>44958</v>
       </c>
       <c r="L5" s="52">
         <f t="shared" si="0"/>
-        <v>44854</v>
+        <v>44959</v>
       </c>
       <c r="M5" s="52">
         <f t="shared" si="0"/>
-        <v>44855</v>
+        <v>44960</v>
       </c>
       <c r="N5" s="52">
         <f t="shared" si="0"/>
-        <v>44856</v>
+        <v>44961</v>
       </c>
       <c r="O5" s="53">
         <f t="shared" si="0"/>
-        <v>44857</v>
+        <v>44962</v>
       </c>
       <c r="P5" s="51">
         <f>O5+1</f>
-        <v>44858</v>
+        <v>44963</v>
       </c>
       <c r="Q5" s="52">
         <f>P5+1</f>
-        <v>44859</v>
+        <v>44964</v>
       </c>
       <c r="R5" s="52">
         <f t="shared" si="0"/>
-        <v>44860</v>
+        <v>44965</v>
       </c>
       <c r="S5" s="52">
         <f t="shared" si="0"/>
-        <v>44861</v>
+        <v>44966</v>
       </c>
       <c r="T5" s="52">
         <f t="shared" si="0"/>
-        <v>44862</v>
+        <v>44967</v>
       </c>
       <c r="U5" s="52">
         <f t="shared" si="0"/>
-        <v>44863</v>
+        <v>44968</v>
       </c>
       <c r="V5" s="53">
         <f t="shared" si="0"/>
-        <v>44864</v>
+        <v>44969</v>
       </c>
       <c r="W5" s="51">
         <f>V5+1</f>
-        <v>44865</v>
+        <v>44970</v>
       </c>
       <c r="X5" s="52">
         <f>W5+1</f>
-        <v>44866</v>
+        <v>44971</v>
       </c>
       <c r="Y5" s="52">
         <f t="shared" si="0"/>
-        <v>44867</v>
+        <v>44972</v>
       </c>
       <c r="Z5" s="52">
         <f t="shared" si="0"/>
-        <v>44868</v>
+        <v>44973</v>
       </c>
       <c r="AA5" s="52">
         <f t="shared" si="0"/>
-        <v>44869</v>
+        <v>44974</v>
       </c>
       <c r="AB5" s="52">
         <f t="shared" si="0"/>
-        <v>44870</v>
+        <v>44975</v>
       </c>
       <c r="AC5" s="53">
         <f t="shared" si="0"/>
-        <v>44871</v>
+        <v>44976</v>
       </c>
       <c r="AD5" s="51">
         <f>AC5+1</f>
-        <v>44872</v>
+        <v>44977</v>
       </c>
       <c r="AE5" s="52">
         <f>AD5+1</f>
-        <v>44873</v>
+        <v>44978</v>
       </c>
       <c r="AF5" s="52">
         <f t="shared" si="0"/>
-        <v>44874</v>
+        <v>44979</v>
       </c>
       <c r="AG5" s="52">
         <f t="shared" si="0"/>
-        <v>44875</v>
+        <v>44980</v>
       </c>
       <c r="AH5" s="52">
         <f t="shared" si="0"/>
-        <v>44876</v>
+        <v>44981</v>
       </c>
       <c r="AI5" s="52">
         <f t="shared" si="0"/>
-        <v>44877</v>
+        <v>44982</v>
       </c>
       <c r="AJ5" s="53">
         <f t="shared" si="0"/>
-        <v>44878</v>
+        <v>44983</v>
       </c>
       <c r="AK5" s="51">
         <f>AJ5+1</f>
-        <v>44879</v>
+        <v>44984</v>
       </c>
       <c r="AL5" s="52">
         <f>AK5+1</f>
-        <v>44880</v>
+        <v>44985</v>
       </c>
       <c r="AM5" s="52">
         <f t="shared" si="0"/>
-        <v>44881</v>
+        <v>44986</v>
       </c>
       <c r="AN5" s="52">
         <f t="shared" si="0"/>
-        <v>44882</v>
+        <v>44987</v>
       </c>
       <c r="AO5" s="52">
         <f t="shared" si="0"/>
-        <v>44883</v>
+        <v>44988</v>
       </c>
       <c r="AP5" s="52">
         <f t="shared" si="0"/>
-        <v>44884</v>
+        <v>44989</v>
       </c>
       <c r="AQ5" s="53">
         <f t="shared" si="0"/>
-        <v>44885</v>
+        <v>44990</v>
       </c>
       <c r="AR5" s="51">
         <f>AQ5+1</f>
-        <v>44886</v>
+        <v>44991</v>
       </c>
       <c r="AS5" s="52">
         <f>AR5+1</f>
-        <v>44887</v>
+        <v>44992</v>
       </c>
       <c r="AT5" s="52">
         <f t="shared" si="0"/>
-        <v>44888</v>
+        <v>44993</v>
       </c>
       <c r="AU5" s="52">
         <f t="shared" si="0"/>
-        <v>44889</v>
+        <v>44994</v>
       </c>
       <c r="AV5" s="52">
         <f t="shared" si="0"/>
-        <v>44890</v>
+        <v>44995</v>
       </c>
       <c r="AW5" s="52">
         <f t="shared" si="0"/>
-        <v>44891</v>
+        <v>44996</v>
       </c>
       <c r="AX5" s="53">
         <f t="shared" si="0"/>
-        <v>44892</v>
+        <v>44997</v>
       </c>
       <c r="AY5" s="51">
         <f>AX5+1</f>
-        <v>44893</v>
+        <v>44998</v>
       </c>
       <c r="AZ5" s="52">
         <f>AY5+1</f>
-        <v>44894</v>
+        <v>44999</v>
       </c>
       <c r="BA5" s="52">
         <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
-        <v>44895</v>
+        <v>45000</v>
       </c>
       <c r="BB5" s="52">
         <f t="shared" si="1"/>
-        <v>44896</v>
+        <v>45001</v>
       </c>
       <c r="BC5" s="52">
         <f t="shared" si="1"/>
-        <v>44897</v>
+        <v>45002</v>
       </c>
       <c r="BD5" s="52">
         <f t="shared" si="1"/>
-        <v>44898</v>
+        <v>45003</v>
       </c>
       <c r="BE5" s="53">
         <f t="shared" si="1"/>
-        <v>44899</v>
+        <v>45004</v>
       </c>
       <c r="BF5" s="51">
         <f>BE5+1</f>
-        <v>44900</v>
+        <v>45005</v>
       </c>
       <c r="BG5" s="52">
         <f>BF5+1</f>
-        <v>44901</v>
+        <v>45006</v>
       </c>
       <c r="BH5" s="52">
         <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
-        <v>44902</v>
+        <v>45007</v>
       </c>
       <c r="BI5" s="52">
         <f t="shared" si="2"/>
-        <v>44903</v>
+        <v>45008</v>
       </c>
       <c r="BJ5" s="52">
         <f t="shared" si="2"/>
-        <v>44904</v>
+        <v>45009</v>
       </c>
       <c r="BK5" s="52">
         <f t="shared" si="2"/>
-        <v>44905</v>
+        <v>45010</v>
       </c>
       <c r="BL5" s="53">
         <f t="shared" si="2"/>
-        <v>44906</v>
+        <v>45011</v>
       </c>
       <c r="BM5" s="51">
         <f>BL5+1</f>
-        <v>44907</v>
+        <v>45012</v>
       </c>
       <c r="BN5" s="52">
         <f>BM5+1</f>
-        <v>44908</v>
+        <v>45013</v>
       </c>
       <c r="BO5" s="52">
         <f t="shared" ref="BO5" si="3">BN5+1</f>
-        <v>44909</v>
+        <v>45014</v>
       </c>
       <c r="BP5" s="52">
         <f t="shared" ref="BP5" si="4">BO5+1</f>
-        <v>44910</v>
+        <v>45015</v>
       </c>
       <c r="BQ5" s="52">
         <f t="shared" ref="BQ5" si="5">BP5+1</f>
-        <v>44911</v>
+        <v>45016</v>
       </c>
       <c r="BR5" s="52">
         <f t="shared" ref="BR5" si="6">BQ5+1</f>
-        <v>44912</v>
+        <v>45017</v>
       </c>
       <c r="BS5" s="53">
         <f t="shared" ref="BS5" si="7">BR5+1</f>
-        <v>44913</v>
+        <v>45018</v>
       </c>
     </row>
     <row r="6" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="96"/>
+      <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="E6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I6" s="8" t="str">
         <f t="shared" ref="I6:AN6" si="8">LEFT(TEXT(I5,"jjj"),1)</f>
@@ -2789,23 +3009,23 @@
         <f t="shared" si="9"/>
         <v>d</v>
       </c>
-      <c r="BM6" s="64" t="str">
+      <c r="BM6" s="8" t="str">
         <f t="shared" si="9"/>
         <v>l</v>
       </c>
-      <c r="BN6" s="64" t="str">
+      <c r="BN6" s="8" t="str">
         <f t="shared" si="9"/>
         <v>m</v>
       </c>
-      <c r="BO6" s="64" t="str">
+      <c r="BO6" s="8" t="str">
         <f t="shared" si="9"/>
         <v>m</v>
       </c>
-      <c r="BP6" s="64" t="str">
+      <c r="BP6" s="8" t="str">
         <f t="shared" si="9"/>
         <v>j</v>
       </c>
-      <c r="BQ6" s="64" t="str">
+      <c r="BQ6" s="8" t="str">
         <f t="shared" si="9"/>
         <v>v</v>
       </c>
@@ -2820,7 +3040,7 @@
     </row>
     <row r="7" spans="1:71" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C7" s="31"/>
       <c r="E7"/>
@@ -2877,27 +3097,27 @@
       <c r="BC7" s="17"/>
       <c r="BD7" s="17"/>
       <c r="BE7" s="17"/>
-      <c r="BF7" s="81"/>
-      <c r="BG7" s="100"/>
-      <c r="BH7" s="81"/>
-      <c r="BI7" s="101"/>
-      <c r="BJ7" s="81"/>
-      <c r="BK7" s="81"/>
+      <c r="BF7" s="17"/>
+      <c r="BG7" s="78"/>
+      <c r="BH7" s="17"/>
+      <c r="BI7" s="79"/>
+      <c r="BJ7" s="17"/>
+      <c r="BK7" s="17"/>
       <c r="BL7" s="17"/>
-      <c r="BM7" s="65"/>
-      <c r="BN7" s="65"/>
-      <c r="BO7" s="65"/>
-      <c r="BP7" s="65"/>
-      <c r="BQ7" s="65"/>
+      <c r="BM7" s="63"/>
+      <c r="BN7" s="63"/>
+      <c r="BO7" s="63"/>
+      <c r="BP7" s="63"/>
+      <c r="BQ7" s="63"/>
       <c r="BR7" s="17"/>
       <c r="BS7" s="17"/>
     </row>
     <row r="8" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="54" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="C8" s="35"/>
       <c r="D8" s="11"/>
@@ -2905,7 +3125,7 @@
       <c r="F8" s="43"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10" t="str">
-        <f t="shared" ref="H8:H27" si="10">IF(OR(ISBLANK(début_tâche),ISBLANK(fin_tâche)),"",fin_tâche-début_tâche+1)</f>
+        <f t="shared" ref="H8:H31" si="10">IF(OR(ISBLANK(début_tâche),ISBLANK(fin_tâche)),"",fin_tâche-début_tâche+1)</f>
         <v/>
       </c>
       <c r="I8" s="17"/>
@@ -2957,42 +3177,42 @@
       <c r="BC8" s="17"/>
       <c r="BD8" s="17"/>
       <c r="BE8" s="17"/>
-      <c r="BF8" s="81"/>
-      <c r="BG8" s="100"/>
-      <c r="BH8" s="81"/>
-      <c r="BI8" s="101"/>
-      <c r="BJ8" s="81"/>
-      <c r="BK8" s="81"/>
+      <c r="BF8" s="17"/>
+      <c r="BG8" s="78"/>
+      <c r="BH8" s="17"/>
+      <c r="BI8" s="79"/>
+      <c r="BJ8" s="17"/>
+      <c r="BK8" s="17"/>
       <c r="BL8" s="17"/>
-      <c r="BM8" s="65"/>
-      <c r="BN8" s="65"/>
-      <c r="BO8" s="65"/>
-      <c r="BP8" s="65"/>
-      <c r="BQ8" s="65"/>
+      <c r="BM8" s="17"/>
+      <c r="BN8" s="17"/>
+      <c r="BO8" s="17"/>
+      <c r="BP8" s="17"/>
+      <c r="BQ8" s="17"/>
       <c r="BR8" s="17"/>
       <c r="BS8" s="17"/>
     </row>
     <row r="9" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="91" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="91"/>
+        <v>15</v>
+      </c>
+      <c r="B9" s="104" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="104"/>
       <c r="D9" s="12">
         <v>1</v>
       </c>
       <c r="E9" s="44">
-        <v>44844</v>
+        <v>44956</v>
       </c>
       <c r="F9" s="44">
-        <v>44890</v>
+        <v>44959</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10">
         <f t="shared" si="10"/>
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
@@ -3043,27 +3263,27 @@
       <c r="BC9" s="17"/>
       <c r="BD9" s="17"/>
       <c r="BE9" s="17"/>
-      <c r="BF9" s="81"/>
-      <c r="BG9" s="100"/>
-      <c r="BH9" s="81"/>
-      <c r="BI9" s="101"/>
-      <c r="BJ9" s="81"/>
-      <c r="BK9" s="81"/>
+      <c r="BF9" s="17"/>
+      <c r="BG9" s="78"/>
+      <c r="BH9" s="17"/>
+      <c r="BI9" s="79"/>
+      <c r="BJ9" s="17"/>
+      <c r="BK9" s="17"/>
       <c r="BL9" s="17"/>
-      <c r="BM9" s="65"/>
-      <c r="BN9" s="65"/>
-      <c r="BO9" s="65"/>
-      <c r="BP9" s="65"/>
-      <c r="BQ9" s="65"/>
+      <c r="BM9" s="17"/>
+      <c r="BN9" s="17"/>
+      <c r="BO9" s="17"/>
+      <c r="BP9" s="17"/>
+      <c r="BQ9" s="17"/>
       <c r="BR9" s="17"/>
       <c r="BS9" s="17"/>
     </row>
     <row r="10" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="11"/>
@@ -3123,42 +3343,42 @@
       <c r="BC10" s="17"/>
       <c r="BD10" s="17"/>
       <c r="BE10" s="17"/>
-      <c r="BF10" s="81"/>
-      <c r="BG10" s="100"/>
-      <c r="BH10" s="81"/>
-      <c r="BI10" s="101"/>
-      <c r="BJ10" s="81"/>
-      <c r="BK10" s="81"/>
+      <c r="BF10" s="17"/>
+      <c r="BG10" s="78"/>
+      <c r="BH10" s="17"/>
+      <c r="BI10" s="79"/>
+      <c r="BJ10" s="17"/>
+      <c r="BK10" s="17"/>
       <c r="BL10" s="17"/>
-      <c r="BM10" s="65"/>
-      <c r="BN10" s="65"/>
-      <c r="BO10" s="65"/>
-      <c r="BP10" s="65"/>
-      <c r="BQ10" s="65"/>
+      <c r="BM10" s="17"/>
+      <c r="BN10" s="17"/>
+      <c r="BO10" s="17"/>
+      <c r="BP10" s="17"/>
+      <c r="BQ10" s="17"/>
       <c r="BR10" s="17"/>
       <c r="BS10" s="17"/>
     </row>
     <row r="11" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="91" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="91"/>
+        <v>15</v>
+      </c>
+      <c r="B11" s="104" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="104"/>
       <c r="D11" s="12">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="E11" s="44">
-        <v>44858</v>
+        <v>44956</v>
       </c>
       <c r="F11" s="44">
-        <v>44899</v>
+        <v>44959</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10">
         <f t="shared" si="10"/>
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
@@ -3209,27 +3429,27 @@
       <c r="BC11" s="17"/>
       <c r="BD11" s="17"/>
       <c r="BE11" s="17"/>
-      <c r="BF11" s="81"/>
-      <c r="BG11" s="100"/>
-      <c r="BH11" s="81"/>
-      <c r="BI11" s="101"/>
-      <c r="BJ11" s="81"/>
-      <c r="BK11" s="81"/>
+      <c r="BF11" s="17"/>
+      <c r="BG11" s="78"/>
+      <c r="BH11" s="17"/>
+      <c r="BI11" s="79"/>
+      <c r="BJ11" s="17"/>
+      <c r="BK11" s="17"/>
       <c r="BL11" s="17"/>
-      <c r="BM11" s="65"/>
-      <c r="BN11" s="65"/>
-      <c r="BO11" s="65"/>
-      <c r="BP11" s="65"/>
-      <c r="BQ11" s="65"/>
+      <c r="BM11" s="17"/>
+      <c r="BN11" s="17"/>
+      <c r="BO11" s="17"/>
+      <c r="BP11" s="17"/>
+      <c r="BQ11" s="17"/>
       <c r="BR11" s="17"/>
       <c r="BS11" s="17"/>
     </row>
     <row r="12" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B12" s="55" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C12" s="36"/>
       <c r="D12" s="13"/>
@@ -3289,40 +3509,40 @@
       <c r="BC12" s="17"/>
       <c r="BD12" s="17"/>
       <c r="BE12" s="17"/>
-      <c r="BF12" s="81"/>
-      <c r="BG12" s="100"/>
-      <c r="BH12" s="81"/>
-      <c r="BI12" s="101"/>
-      <c r="BJ12" s="81"/>
-      <c r="BK12" s="81"/>
+      <c r="BF12" s="17"/>
+      <c r="BG12" s="78"/>
+      <c r="BH12" s="17"/>
+      <c r="BI12" s="79"/>
+      <c r="BJ12" s="17"/>
+      <c r="BK12" s="17"/>
       <c r="BL12" s="17"/>
-      <c r="BM12" s="65"/>
-      <c r="BN12" s="65"/>
-      <c r="BO12" s="65"/>
-      <c r="BP12" s="65"/>
-      <c r="BQ12" s="65"/>
+      <c r="BM12" s="17"/>
+      <c r="BN12" s="17"/>
+      <c r="BO12" s="17"/>
+      <c r="BP12" s="17"/>
+      <c r="BQ12" s="17"/>
       <c r="BR12" s="17"/>
       <c r="BS12" s="17"/>
     </row>
     <row r="13" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
-      <c r="B13" s="92" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="93"/>
+      <c r="B13" s="105" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="106"/>
       <c r="D13" s="14">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="E13" s="47">
-        <v>44876</v>
+        <v>44956</v>
       </c>
       <c r="F13" s="47">
-        <v>44905</v>
+        <v>44959</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10">
         <f t="shared" si="10"/>
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
@@ -3373,27 +3593,27 @@
       <c r="BC13" s="17"/>
       <c r="BD13" s="17"/>
       <c r="BE13" s="17"/>
-      <c r="BF13" s="81"/>
-      <c r="BG13" s="100"/>
-      <c r="BH13" s="81"/>
-      <c r="BI13" s="101"/>
-      <c r="BJ13" s="81"/>
-      <c r="BK13" s="81"/>
+      <c r="BF13" s="17"/>
+      <c r="BG13" s="78"/>
+      <c r="BH13" s="17"/>
+      <c r="BI13" s="79"/>
+      <c r="BJ13" s="17"/>
+      <c r="BK13" s="17"/>
       <c r="BL13" s="17"/>
-      <c r="BM13" s="65"/>
-      <c r="BN13" s="65"/>
-      <c r="BO13" s="65"/>
-      <c r="BP13" s="65"/>
-      <c r="BQ13" s="65"/>
+      <c r="BM13" s="17"/>
+      <c r="BN13" s="17"/>
+      <c r="BO13" s="17"/>
+      <c r="BP13" s="17"/>
+      <c r="BQ13" s="17"/>
       <c r="BR13" s="17"/>
       <c r="BS13" s="17"/>
     </row>
     <row r="14" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C14" s="37"/>
       <c r="D14" s="15"/>
@@ -3453,40 +3673,40 @@
       <c r="BC14" s="17"/>
       <c r="BD14" s="17"/>
       <c r="BE14" s="17"/>
-      <c r="BF14" s="81"/>
-      <c r="BG14" s="100"/>
-      <c r="BH14" s="81"/>
-      <c r="BI14" s="101"/>
-      <c r="BJ14" s="81"/>
-      <c r="BK14" s="81"/>
+      <c r="BF14" s="17"/>
+      <c r="BG14" s="78"/>
+      <c r="BH14" s="17"/>
+      <c r="BI14" s="79"/>
+      <c r="BJ14" s="17"/>
+      <c r="BK14" s="17"/>
       <c r="BL14" s="17"/>
-      <c r="BM14" s="65"/>
-      <c r="BN14" s="65"/>
-      <c r="BO14" s="65"/>
-      <c r="BP14" s="65"/>
-      <c r="BQ14" s="65"/>
+      <c r="BM14" s="17"/>
+      <c r="BN14" s="17"/>
+      <c r="BO14" s="17"/>
+      <c r="BP14" s="17"/>
+      <c r="BQ14" s="17"/>
       <c r="BR14" s="17"/>
       <c r="BS14" s="17"/>
     </row>
     <row r="15" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
-      <c r="B15" s="89" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="90"/>
+      <c r="B15" s="102" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="103"/>
       <c r="D15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="50">
-        <v>44883</v>
+        <v>44956</v>
       </c>
       <c r="F15" s="50">
-        <v>44909</v>
+        <v>44959</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
@@ -3537,27 +3757,27 @@
       <c r="BC15" s="17"/>
       <c r="BD15" s="17"/>
       <c r="BE15" s="17"/>
-      <c r="BF15" s="81"/>
-      <c r="BG15" s="100"/>
-      <c r="BH15" s="81"/>
-      <c r="BI15" s="101"/>
-      <c r="BJ15" s="81"/>
-      <c r="BK15" s="81"/>
+      <c r="BF15" s="17"/>
+      <c r="BG15" s="78"/>
+      <c r="BH15" s="17"/>
+      <c r="BI15" s="79"/>
+      <c r="BJ15" s="17"/>
+      <c r="BK15" s="17"/>
       <c r="BL15" s="17"/>
-      <c r="BM15" s="65"/>
-      <c r="BN15" s="65"/>
-      <c r="BO15" s="65"/>
-      <c r="BP15" s="65"/>
-      <c r="BQ15" s="65"/>
+      <c r="BM15" s="17"/>
+      <c r="BN15" s="17"/>
+      <c r="BO15" s="17"/>
+      <c r="BP15" s="17"/>
+      <c r="BQ15" s="17"/>
       <c r="BR15" s="17"/>
       <c r="BS15" s="17"/>
     </row>
     <row r="16" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B16" s="56" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C16" s="37"/>
       <c r="D16" s="15"/>
@@ -3617,29 +3837,29 @@
       <c r="BC16" s="17"/>
       <c r="BD16" s="17"/>
       <c r="BE16" s="17"/>
-      <c r="BF16" s="81"/>
-      <c r="BG16" s="100"/>
-      <c r="BH16" s="81"/>
-      <c r="BI16" s="101"/>
-      <c r="BJ16" s="81"/>
-      <c r="BK16" s="81"/>
+      <c r="BF16" s="17"/>
+      <c r="BG16" s="78"/>
+      <c r="BH16" s="17"/>
+      <c r="BI16" s="79"/>
+      <c r="BJ16" s="17"/>
+      <c r="BK16" s="17"/>
       <c r="BL16" s="17"/>
-      <c r="BM16" s="65"/>
-      <c r="BN16" s="65"/>
-      <c r="BO16" s="65"/>
-      <c r="BP16" s="65"/>
-      <c r="BQ16" s="65"/>
+      <c r="BM16" s="17"/>
+      <c r="BN16" s="17"/>
+      <c r="BO16" s="17"/>
+      <c r="BP16" s="17"/>
+      <c r="BQ16" s="17"/>
       <c r="BR16" s="17"/>
       <c r="BS16" s="17"/>
     </row>
     <row r="17" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
-      <c r="B17" s="89" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="90"/>
+      <c r="B17" s="102" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="103"/>
       <c r="D17" s="16">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E17" s="50">
         <v>44890</v>
@@ -3702,27 +3922,27 @@
       <c r="BC17" s="17"/>
       <c r="BD17" s="17"/>
       <c r="BE17" s="17"/>
-      <c r="BF17" s="81"/>
-      <c r="BG17" s="100"/>
-      <c r="BH17" s="81"/>
-      <c r="BI17" s="101"/>
-      <c r="BJ17" s="81"/>
-      <c r="BK17" s="81"/>
+      <c r="BF17" s="17"/>
+      <c r="BG17" s="78"/>
+      <c r="BH17" s="17"/>
+      <c r="BI17" s="79"/>
+      <c r="BJ17" s="17"/>
+      <c r="BK17" s="17"/>
       <c r="BL17" s="17"/>
-      <c r="BM17" s="65"/>
-      <c r="BN17" s="65"/>
-      <c r="BO17" s="65"/>
-      <c r="BP17" s="65"/>
-      <c r="BQ17" s="65"/>
+      <c r="BM17" s="17"/>
+      <c r="BN17" s="17"/>
+      <c r="BO17" s="17"/>
+      <c r="BP17" s="17"/>
+      <c r="BQ17" s="17"/>
       <c r="BR17" s="17"/>
       <c r="BS17" s="17"/>
     </row>
     <row r="18" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B18" s="56" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="15"/>
@@ -3782,40 +4002,40 @@
       <c r="BC18" s="17"/>
       <c r="BD18" s="17"/>
       <c r="BE18" s="17"/>
-      <c r="BF18" s="81"/>
-      <c r="BG18" s="100"/>
-      <c r="BH18" s="81"/>
-      <c r="BI18" s="101"/>
-      <c r="BJ18" s="81"/>
-      <c r="BK18" s="81"/>
+      <c r="BF18" s="17"/>
+      <c r="BG18" s="78"/>
+      <c r="BH18" s="17"/>
+      <c r="BI18" s="79"/>
+      <c r="BJ18" s="17"/>
+      <c r="BK18" s="17"/>
       <c r="BL18" s="17"/>
-      <c r="BM18" s="65"/>
-      <c r="BN18" s="65"/>
-      <c r="BO18" s="65"/>
-      <c r="BP18" s="65"/>
-      <c r="BQ18" s="65"/>
+      <c r="BM18" s="17"/>
+      <c r="BN18" s="17"/>
+      <c r="BO18" s="17"/>
+      <c r="BP18" s="17"/>
+      <c r="BQ18" s="17"/>
       <c r="BR18" s="17"/>
       <c r="BS18" s="17"/>
     </row>
     <row r="19" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
-      <c r="B19" s="89" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="90"/>
+      <c r="B19" s="109" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="110"/>
       <c r="D19" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="50">
-        <v>44876</v>
+        <v>44959</v>
       </c>
       <c r="F19" s="50">
-        <v>44890</v>
+        <v>45007</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10">
         <f t="shared" si="10"/>
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
@@ -3866,32 +4086,32 @@
       <c r="BC19" s="17"/>
       <c r="BD19" s="17"/>
       <c r="BE19" s="17"/>
-      <c r="BF19" s="81"/>
-      <c r="BG19" s="100"/>
-      <c r="BH19" s="81"/>
-      <c r="BI19" s="101"/>
-      <c r="BJ19" s="81"/>
-      <c r="BK19" s="81"/>
+      <c r="BF19" s="17"/>
+      <c r="BG19" s="78"/>
+      <c r="BH19" s="17"/>
+      <c r="BI19" s="79"/>
+      <c r="BJ19" s="17"/>
+      <c r="BK19" s="17"/>
       <c r="BL19" s="17"/>
-      <c r="BM19" s="65"/>
-      <c r="BN19" s="65"/>
-      <c r="BO19" s="65"/>
-      <c r="BP19" s="65"/>
-      <c r="BQ19" s="65"/>
+      <c r="BM19" s="17"/>
+      <c r="BN19" s="17"/>
+      <c r="BO19" s="17"/>
+      <c r="BP19" s="17"/>
+      <c r="BQ19" s="17"/>
       <c r="BR19" s="17"/>
       <c r="BS19" s="17"/>
     </row>
     <row r="20" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="67"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="70"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="80"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="67"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10" t="str">
         <f t="shared" si="10"/>
@@ -3946,42 +4166,42 @@
       <c r="BC20" s="17"/>
       <c r="BD20" s="17"/>
       <c r="BE20" s="17"/>
-      <c r="BF20" s="81"/>
-      <c r="BG20" s="100"/>
-      <c r="BH20" s="81"/>
-      <c r="BI20" s="101"/>
-      <c r="BJ20" s="81"/>
-      <c r="BK20" s="81"/>
+      <c r="BF20" s="17"/>
+      <c r="BG20" s="78"/>
+      <c r="BH20" s="17"/>
+      <c r="BI20" s="79"/>
+      <c r="BJ20" s="17"/>
+      <c r="BK20" s="17"/>
       <c r="BL20" s="17"/>
-      <c r="BM20" s="65"/>
-      <c r="BN20" s="65"/>
-      <c r="BO20" s="65"/>
-      <c r="BP20" s="65"/>
-      <c r="BQ20" s="65"/>
+      <c r="BM20" s="17"/>
+      <c r="BN20" s="17"/>
+      <c r="BO20" s="17"/>
+      <c r="BP20" s="17"/>
+      <c r="BQ20" s="17"/>
       <c r="BR20" s="17"/>
       <c r="BS20" s="17"/>
     </row>
     <row r="21" spans="1:71" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="72">
-        <v>0.25</v>
-      </c>
-      <c r="E21" s="73">
-        <v>44890</v>
-      </c>
-      <c r="F21" s="73">
-        <v>44905</v>
+      <c r="B21" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="81"/>
+      <c r="D21" s="69">
+        <v>0</v>
+      </c>
+      <c r="E21" s="70">
+        <v>44959</v>
+      </c>
+      <c r="F21" s="70">
+        <v>45079</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10">
         <f t="shared" si="10"/>
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
@@ -4032,29 +4252,29 @@
       <c r="BC21" s="17"/>
       <c r="BD21" s="17"/>
       <c r="BE21" s="17"/>
-      <c r="BF21" s="81"/>
-      <c r="BG21" s="100"/>
-      <c r="BH21" s="81"/>
-      <c r="BI21" s="101"/>
-      <c r="BJ21" s="81"/>
-      <c r="BK21" s="81"/>
+      <c r="BF21" s="17"/>
+      <c r="BG21" s="78"/>
+      <c r="BH21" s="17"/>
+      <c r="BI21" s="79"/>
+      <c r="BJ21" s="17"/>
+      <c r="BK21" s="17"/>
       <c r="BL21" s="17"/>
-      <c r="BM21" s="65"/>
-      <c r="BN21" s="65"/>
-      <c r="BO21" s="65"/>
-      <c r="BP21" s="65"/>
-      <c r="BQ21" s="65"/>
+      <c r="BM21" s="17"/>
+      <c r="BN21" s="17"/>
+      <c r="BO21" s="17"/>
+      <c r="BP21" s="17"/>
+      <c r="BQ21" s="17"/>
       <c r="BR21" s="17"/>
       <c r="BS21" s="17"/>
     </row>
     <row r="22" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="67"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="70"/>
+      <c r="B22" s="68" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="80"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="67"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10" t="str">
         <f t="shared" si="10"/>
@@ -4109,39 +4329,39 @@
       <c r="BC22" s="17"/>
       <c r="BD22" s="17"/>
       <c r="BE22" s="17"/>
-      <c r="BF22" s="81"/>
-      <c r="BG22" s="100"/>
-      <c r="BH22" s="81"/>
-      <c r="BI22" s="101"/>
-      <c r="BJ22" s="81"/>
-      <c r="BK22" s="81"/>
+      <c r="BF22" s="17"/>
+      <c r="BG22" s="78"/>
+      <c r="BH22" s="17"/>
+      <c r="BI22" s="79"/>
+      <c r="BJ22" s="17"/>
+      <c r="BK22" s="17"/>
       <c r="BL22" s="17"/>
-      <c r="BM22" s="65"/>
-      <c r="BN22" s="65"/>
-      <c r="BO22" s="65"/>
-      <c r="BP22" s="65"/>
-      <c r="BQ22" s="65"/>
+      <c r="BM22" s="17"/>
+      <c r="BN22" s="17"/>
+      <c r="BO22" s="17"/>
+      <c r="BP22" s="17"/>
+      <c r="BQ22" s="17"/>
       <c r="BR22" s="17"/>
       <c r="BS22" s="17"/>
     </row>
     <row r="23" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="82" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="83"/>
-      <c r="D23" s="72">
-        <v>0.3</v>
-      </c>
-      <c r="E23" s="73">
-        <v>44902</v>
-      </c>
-      <c r="F23" s="73">
-        <v>44911</v>
+      <c r="B23" s="83" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="81"/>
+      <c r="D23" s="69">
+        <v>0</v>
+      </c>
+      <c r="E23" s="70">
+        <v>44959</v>
+      </c>
+      <c r="F23" s="70">
+        <v>45201</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>243</v>
       </c>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
@@ -4192,29 +4412,29 @@
       <c r="BC23" s="17"/>
       <c r="BD23" s="17"/>
       <c r="BE23" s="17"/>
-      <c r="BF23" s="81"/>
-      <c r="BG23" s="100"/>
-      <c r="BH23" s="81"/>
-      <c r="BI23" s="101"/>
-      <c r="BJ23" s="81"/>
-      <c r="BK23" s="81"/>
+      <c r="BF23" s="17"/>
+      <c r="BG23" s="78"/>
+      <c r="BH23" s="17"/>
+      <c r="BI23" s="79"/>
+      <c r="BJ23" s="17"/>
+      <c r="BK23" s="17"/>
       <c r="BL23" s="17"/>
-      <c r="BM23" s="65"/>
-      <c r="BN23" s="65"/>
-      <c r="BO23" s="65"/>
-      <c r="BP23" s="65"/>
-      <c r="BQ23" s="65"/>
+      <c r="BM23" s="17"/>
+      <c r="BN23" s="17"/>
+      <c r="BO23" s="17"/>
+      <c r="BP23" s="17"/>
+      <c r="BQ23" s="17"/>
       <c r="BR23" s="17"/>
       <c r="BS23" s="17"/>
     </row>
     <row r="24" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="60"/>
+      <c r="B24" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="82"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="59"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
       <c r="I24" s="17"/>
@@ -4266,39 +4486,39 @@
       <c r="BC24" s="17"/>
       <c r="BD24" s="17"/>
       <c r="BE24" s="17"/>
-      <c r="BF24" s="81"/>
-      <c r="BG24" s="100"/>
-      <c r="BH24" s="81"/>
-      <c r="BI24" s="101"/>
-      <c r="BJ24" s="81"/>
-      <c r="BK24" s="81"/>
+      <c r="BF24" s="17"/>
+      <c r="BG24" s="78"/>
+      <c r="BH24" s="17"/>
+      <c r="BI24" s="79"/>
+      <c r="BJ24" s="17"/>
+      <c r="BK24" s="17"/>
       <c r="BL24" s="17"/>
-      <c r="BM24" s="65"/>
-      <c r="BN24" s="65"/>
-      <c r="BO24" s="65"/>
-      <c r="BP24" s="65"/>
-      <c r="BQ24" s="65"/>
+      <c r="BM24" s="17"/>
+      <c r="BN24" s="17"/>
+      <c r="BO24" s="17"/>
+      <c r="BP24" s="17"/>
+      <c r="BQ24" s="17"/>
       <c r="BR24" s="17"/>
       <c r="BS24" s="17"/>
     </row>
     <row r="25" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="94" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="95"/>
-      <c r="D25" s="61">
+      <c r="B25" s="107" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="108"/>
+      <c r="D25" s="60">
         <v>0</v>
       </c>
-      <c r="E25" s="62">
-        <v>44897</v>
-      </c>
-      <c r="F25" s="62">
-        <v>44906</v>
+      <c r="E25" s="61">
+        <v>44959</v>
+      </c>
+      <c r="F25" s="61" t="s">
+        <v>45</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
@@ -4349,29 +4569,29 @@
       <c r="BC25" s="17"/>
       <c r="BD25" s="17"/>
       <c r="BE25" s="17"/>
-      <c r="BF25" s="81"/>
-      <c r="BG25" s="100"/>
-      <c r="BH25" s="81"/>
-      <c r="BI25" s="101"/>
-      <c r="BJ25" s="81"/>
-      <c r="BK25" s="81"/>
+      <c r="BF25" s="17"/>
+      <c r="BG25" s="78"/>
+      <c r="BH25" s="17"/>
+      <c r="BI25" s="79"/>
+      <c r="BJ25" s="17"/>
+      <c r="BK25" s="17"/>
       <c r="BL25" s="17"/>
-      <c r="BM25" s="65"/>
-      <c r="BN25" s="65"/>
-      <c r="BO25" s="65"/>
-      <c r="BP25" s="65"/>
-      <c r="BQ25" s="65"/>
+      <c r="BM25" s="17"/>
+      <c r="BN25" s="17"/>
+      <c r="BO25" s="17"/>
+      <c r="BP25" s="17"/>
+      <c r="BQ25" s="17"/>
       <c r="BR25" s="17"/>
       <c r="BS25" s="17"/>
     </row>
     <row r="26" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="74" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="75"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="78"/>
+      <c r="B26" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="72"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="75"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
       <c r="I26" s="17"/>
@@ -4423,39 +4643,39 @@
       <c r="BC26" s="17"/>
       <c r="BD26" s="17"/>
       <c r="BE26" s="17"/>
-      <c r="BF26" s="81"/>
-      <c r="BG26" s="100"/>
-      <c r="BH26" s="81"/>
-      <c r="BI26" s="101"/>
-      <c r="BJ26" s="81"/>
-      <c r="BK26" s="81"/>
+      <c r="BF26" s="17"/>
+      <c r="BG26" s="78"/>
+      <c r="BH26" s="17"/>
+      <c r="BI26" s="79"/>
+      <c r="BJ26" s="17"/>
+      <c r="BK26" s="17"/>
       <c r="BL26" s="17"/>
-      <c r="BM26" s="65"/>
-      <c r="BN26" s="65"/>
-      <c r="BO26" s="65"/>
-      <c r="BP26" s="65"/>
-      <c r="BQ26" s="65"/>
+      <c r="BM26" s="17"/>
+      <c r="BN26" s="17"/>
+      <c r="BO26" s="17"/>
+      <c r="BP26" s="17"/>
+      <c r="BQ26" s="17"/>
       <c r="BR26" s="17"/>
       <c r="BS26" s="17"/>
     </row>
     <row r="27" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="87" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="88"/>
-      <c r="D27" s="79">
+      <c r="B27" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="101"/>
+      <c r="D27" s="76">
         <v>0</v>
       </c>
-      <c r="E27" s="80">
-        <v>44907</v>
-      </c>
-      <c r="F27" s="80">
-        <v>44911</v>
+      <c r="E27" s="77">
+        <v>45000</v>
+      </c>
+      <c r="F27" s="77">
+        <v>45005</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="10">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
@@ -4506,36 +4726,339 @@
       <c r="BC27" s="17"/>
       <c r="BD27" s="17"/>
       <c r="BE27" s="17"/>
-      <c r="BF27" s="81"/>
-      <c r="BG27" s="100"/>
-      <c r="BH27" s="81"/>
-      <c r="BI27" s="101"/>
-      <c r="BJ27" s="81"/>
-      <c r="BK27" s="81"/>
+      <c r="BF27" s="17"/>
+      <c r="BG27" s="78"/>
+      <c r="BH27" s="17"/>
+      <c r="BI27" s="79"/>
+      <c r="BJ27" s="17"/>
+      <c r="BK27" s="17"/>
       <c r="BL27" s="17"/>
-      <c r="BM27" s="65"/>
-      <c r="BN27" s="65"/>
-      <c r="BO27" s="65"/>
-      <c r="BP27" s="65"/>
-      <c r="BQ27" s="65"/>
+      <c r="BM27" s="17"/>
+      <c r="BN27" s="17"/>
+      <c r="BO27" s="17"/>
+      <c r="BP27" s="17"/>
+      <c r="BQ27" s="17"/>
       <c r="BR27" s="17"/>
       <c r="BS27" s="17"/>
     </row>
-    <row r="28" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="9"/>
+    <row r="28" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="72"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="17"/>
+      <c r="AE28" s="17"/>
+      <c r="AF28" s="17"/>
+      <c r="AG28" s="17"/>
+      <c r="AH28" s="17"/>
+      <c r="AI28" s="17"/>
+      <c r="AJ28" s="17"/>
+      <c r="AK28" s="17"/>
+      <c r="AL28" s="17"/>
+      <c r="AM28" s="17"/>
+      <c r="AN28" s="17"/>
+      <c r="AO28" s="17"/>
+      <c r="AP28" s="17"/>
+      <c r="AQ28" s="17"/>
+      <c r="AR28" s="17"/>
+      <c r="AS28" s="17"/>
+      <c r="AT28" s="17"/>
+      <c r="AU28" s="17"/>
+      <c r="AV28" s="17"/>
+      <c r="AW28" s="17"/>
+      <c r="AX28" s="17"/>
+      <c r="AY28" s="17"/>
+      <c r="AZ28" s="17"/>
+      <c r="BA28" s="17"/>
+      <c r="BB28" s="17"/>
+      <c r="BC28" s="17"/>
+      <c r="BD28" s="17"/>
+      <c r="BE28" s="17"/>
+      <c r="BF28" s="17"/>
+      <c r="BG28" s="78"/>
+      <c r="BH28" s="17"/>
+      <c r="BI28" s="79"/>
+      <c r="BJ28" s="17"/>
+      <c r="BK28" s="17"/>
+      <c r="BL28" s="17"/>
+      <c r="BM28" s="17"/>
+      <c r="BN28" s="17"/>
+      <c r="BO28" s="17"/>
+      <c r="BP28" s="17"/>
+      <c r="BQ28" s="17"/>
+      <c r="BR28" s="17"/>
+      <c r="BS28" s="17"/>
+    </row>
+    <row r="29" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="101"/>
+      <c r="D29" s="76">
+        <v>0</v>
+      </c>
+      <c r="E29" s="77">
+        <v>45000</v>
+      </c>
+      <c r="F29" s="77">
+        <v>45005</v>
+      </c>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+      <c r="Y29" s="17"/>
+      <c r="Z29" s="17"/>
+      <c r="AA29" s="17"/>
+      <c r="AB29" s="17"/>
+      <c r="AC29" s="17"/>
+      <c r="AD29" s="17"/>
+      <c r="AE29" s="17"/>
+      <c r="AF29" s="17"/>
+      <c r="AG29" s="17"/>
+      <c r="AH29" s="17"/>
+      <c r="AI29" s="17"/>
+      <c r="AJ29" s="17"/>
+      <c r="AK29" s="17"/>
+      <c r="AL29" s="17"/>
+      <c r="AM29" s="17"/>
+      <c r="AN29" s="17"/>
+      <c r="AO29" s="17"/>
+      <c r="AP29" s="17"/>
+      <c r="AQ29" s="17"/>
+      <c r="AR29" s="17"/>
+      <c r="AS29" s="17"/>
+      <c r="AT29" s="17"/>
+      <c r="AU29" s="17"/>
+      <c r="AV29" s="17"/>
+      <c r="AW29" s="17"/>
+      <c r="AX29" s="17"/>
+      <c r="AY29" s="17"/>
+      <c r="AZ29" s="17"/>
+      <c r="BA29" s="17"/>
+      <c r="BB29" s="17"/>
+      <c r="BC29" s="17"/>
+      <c r="BD29" s="17"/>
+      <c r="BE29" s="17"/>
+      <c r="BF29" s="17"/>
+      <c r="BG29" s="78"/>
+      <c r="BH29" s="17"/>
+      <c r="BI29" s="79"/>
+      <c r="BJ29" s="17"/>
+      <c r="BK29" s="17"/>
+      <c r="BL29" s="17"/>
+      <c r="BM29" s="17"/>
+      <c r="BN29" s="17"/>
+      <c r="BO29" s="17"/>
+      <c r="BP29" s="17"/>
+      <c r="BQ29" s="17"/>
+      <c r="BR29" s="17"/>
+      <c r="BS29" s="17"/>
+    </row>
+    <row r="30" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="84" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="85"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="17"/>
+      <c r="AA30" s="17"/>
+      <c r="AB30" s="17"/>
+      <c r="AC30" s="17"/>
+      <c r="AD30" s="17"/>
+      <c r="AE30" s="17"/>
+      <c r="AF30" s="17"/>
+      <c r="AG30" s="17"/>
+      <c r="AH30" s="17"/>
+      <c r="AI30" s="17"/>
+      <c r="AJ30" s="17"/>
+      <c r="AK30" s="17"/>
+      <c r="AL30" s="17"/>
+      <c r="AM30" s="17"/>
+      <c r="AN30" s="17"/>
+      <c r="AO30" s="17"/>
+      <c r="AP30" s="17"/>
+      <c r="AQ30" s="17"/>
+      <c r="AR30" s="17"/>
+      <c r="AS30" s="17"/>
+      <c r="AT30" s="17"/>
+      <c r="AU30" s="17"/>
+      <c r="AV30" s="17"/>
+      <c r="AW30" s="17"/>
+      <c r="AX30" s="17"/>
+      <c r="AY30" s="17"/>
+      <c r="AZ30" s="17"/>
+      <c r="BA30" s="17"/>
+      <c r="BB30" s="17"/>
+      <c r="BC30" s="17"/>
+      <c r="BD30" s="17"/>
+      <c r="BE30" s="17"/>
+      <c r="BF30" s="17"/>
+      <c r="BG30" s="78"/>
+      <c r="BH30" s="17"/>
+      <c r="BI30" s="79"/>
+      <c r="BJ30" s="17"/>
+      <c r="BK30" s="17"/>
+      <c r="BL30" s="17"/>
+      <c r="BM30" s="17"/>
+      <c r="BN30" s="17"/>
+      <c r="BO30" s="17"/>
+      <c r="BP30" s="17"/>
+      <c r="BQ30" s="17"/>
+      <c r="BR30" s="17"/>
+      <c r="BS30" s="17"/>
+    </row>
+    <row r="31" spans="1:71" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="98" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="99"/>
+      <c r="D31" s="89">
+        <v>0</v>
+      </c>
+      <c r="E31" s="90"/>
+      <c r="F31" s="90"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+      <c r="AA31" s="17"/>
+      <c r="AB31" s="17"/>
+      <c r="AC31" s="17"/>
+      <c r="AD31" s="17"/>
+      <c r="AE31" s="17"/>
+      <c r="AF31" s="17"/>
+      <c r="AG31" s="17"/>
+      <c r="AH31" s="17"/>
+      <c r="AI31" s="17"/>
+      <c r="AJ31" s="17"/>
+      <c r="AK31" s="17"/>
+      <c r="AL31" s="17"/>
+      <c r="AM31" s="17"/>
+      <c r="AN31" s="17"/>
+      <c r="AO31" s="17"/>
+      <c r="AP31" s="17"/>
+      <c r="AQ31" s="17"/>
+      <c r="AR31" s="17"/>
+      <c r="AS31" s="17"/>
+      <c r="AT31" s="17"/>
+      <c r="AU31" s="17"/>
+      <c r="AV31" s="17"/>
+      <c r="AW31" s="17"/>
+      <c r="AX31" s="17"/>
+      <c r="AY31" s="17"/>
+      <c r="AZ31" s="17"/>
+      <c r="BA31" s="17"/>
+      <c r="BB31" s="17"/>
+      <c r="BC31" s="17"/>
+      <c r="BD31" s="17"/>
+      <c r="BE31" s="17"/>
+      <c r="BF31" s="17"/>
+      <c r="BG31" s="78"/>
+      <c r="BH31" s="17"/>
+      <c r="BI31" s="79"/>
+      <c r="BJ31" s="17"/>
+      <c r="BK31" s="17"/>
+      <c r="BL31" s="17"/>
+      <c r="BM31" s="17"/>
+      <c r="BN31" s="17"/>
+      <c r="BO31" s="17"/>
+      <c r="BP31" s="17"/>
+      <c r="BQ31" s="17"/>
+      <c r="BR31" s="17"/>
+      <c r="BS31" s="17"/>
+    </row>
+    <row r="32" spans="1:71" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="B21:C21"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B9:C9"/>
@@ -4549,9 +5072,16 @@
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="AD4:AJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D27">
-    <cfRule type="dataBar" priority="25">
+  <conditionalFormatting sqref="D7:D19 D26:D31">
+    <cfRule type="dataBar" priority="47">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -4564,75 +5094,209 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL5 I7:BG21 BL6 BI7:BL21 BH7:BH27 I6:BJ6">
-    <cfRule type="expression" dxfId="13" priority="44">
+  <conditionalFormatting sqref="I5:BL5 I7:BG21 BI7:BL21 I6:BJ6 BH7:BH31 BL6:BQ6">
+    <cfRule type="expression" dxfId="31" priority="66">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BG21 BI7:BL21 BH7:BH27">
-    <cfRule type="expression" dxfId="12" priority="38">
+  <conditionalFormatting sqref="I7:BG21 BI7:BL21 BH7:BH31">
+    <cfRule type="expression" dxfId="30" priority="60">
       <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="61" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:BG27 BI22:BL27">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="28" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I22:BG27 BI22:BL27">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="27" priority="31">
       <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="32" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM5:BS5 BM7:BS21 BS6">
-    <cfRule type="expression" dxfId="7" priority="8">
+  <conditionalFormatting sqref="BM5:BS5 BM7:BS7 BS6 BR8:BS21">
+    <cfRule type="expression" dxfId="25" priority="30">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM7:BS21">
-    <cfRule type="expression" dxfId="6" priority="6">
+  <conditionalFormatting sqref="BM7:BS7 BR8:BS21">
+    <cfRule type="expression" dxfId="24" priority="28">
       <formula>AND(début_tâche&lt;=BM$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=BM$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="29" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=BM$5,début_tâche&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM22:BS27">
-    <cfRule type="expression" dxfId="4" priority="5">
+  <conditionalFormatting sqref="BR22:BS27">
+    <cfRule type="expression" dxfId="22" priority="27">
+      <formula>AND(TODAY()&gt;=BR$5,TODAY()&lt;BS$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BR22:BS27">
+    <cfRule type="expression" dxfId="21" priority="25">
+      <formula>AND(début_tâche&lt;=BR$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=BR$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="26" stopIfTrue="1">
+      <formula>AND(fin_tâche&gt;=BR$5,début_tâche&lt;BS$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BR6">
+    <cfRule type="expression" dxfId="19" priority="24">
+      <formula>AND(TODAY()&gt;=BR$5,TODAY()&lt;BS$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BK6">
+    <cfRule type="expression" dxfId="18" priority="23">
+      <formula>AND(TODAY()&gt;=BK$5,TODAY()&lt;BL$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:D23">
+    <cfRule type="dataBar" priority="22">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{76330665-AA93-4150-A7E6-6D0D1A0B20EF}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B21:C21">
+    <cfRule type="dataBar" priority="21">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7FA9031D-5489-4F15-BD46-DEFB64E198FC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:C23">
+    <cfRule type="dataBar" priority="20">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DF5CD11B-1EFF-4C24-B7C3-2E4277F3C896}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24:D25">
+    <cfRule type="dataBar" priority="19">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{85DE7253-C4BE-4E02-B679-A25AB6B6323C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30:BG31 BI30:BL31">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I30:BG31 BI30:BL31">
+    <cfRule type="expression" dxfId="16" priority="16">
+      <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
+      <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BR30:BS31">
+    <cfRule type="expression" dxfId="14" priority="15">
+      <formula>AND(TODAY()&gt;=BR$5,TODAY()&lt;BS$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BR30:BS31">
+    <cfRule type="expression" dxfId="13" priority="13">
+      <formula>AND(début_tâche&lt;=BR$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=BR$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
+      <formula>AND(fin_tâche&gt;=BR$5,début_tâche&lt;BS$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28:BG29 BI28:BL29">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I28:BG29 BI28:BL29">
+    <cfRule type="expression" dxfId="10" priority="10">
+      <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
+      <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BR28:BS29">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>AND(TODAY()&gt;=BR$5,TODAY()&lt;BS$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BR28:BS29">
+    <cfRule type="expression" dxfId="7" priority="7">
+      <formula>AND(début_tâche&lt;=BR$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=BR$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+      <formula>AND(fin_tâche&gt;=BR$5,début_tâche&lt;BS$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM8:BQ8 BM10:BQ10 BM12:BQ12 BM14:BQ14 BM16:BQ16 BM18:BQ18 BM20:BQ20 BM22:BQ22 BM24:BQ24 BM26:BQ26 BM28:BQ28 BM30:BQ30">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM22:BS27">
-    <cfRule type="expression" dxfId="3" priority="3">
+  <conditionalFormatting sqref="BM8:BQ8 BM10:BQ10 BM12:BQ12 BM14:BQ14 BM16:BQ16 BM18:BQ18 BM20:BQ20 BM22:BQ22 BM24:BQ24 BM26:BQ26 BM28:BQ28 BM30:BQ30">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>AND(début_tâche&lt;=BM$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=BM$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=BM$5,début_tâche&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM6:BR6">
-    <cfRule type="expression" dxfId="1" priority="2">
+  <conditionalFormatting sqref="BM9:BQ9 BM11:BQ11 BM13:BQ13 BM15:BQ15 BM17:BQ17 BM19:BQ19 BM21:BQ21 BM23:BQ23 BM25:BQ25 BM27:BQ27 BM29:BQ29 BM31:BQ31">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND(TODAY()&gt;=BM$5,TODAY()&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BK6">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(TODAY()&gt;=BK$5,TODAY()&lt;BL$5)</formula>
+  <conditionalFormatting sqref="BM9:BQ9 BM11:BQ11 BM13:BQ13 BM15:BQ15 BM17:BQ17 BM19:BQ19 BM21:BQ21 BM23:BQ23 BM25:BQ25 BM27:BQ27 BM29:BQ29 BM31:BQ31">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND(début_tâche&lt;=BM$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=BM$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>AND(fin_tâche&gt;=BM$5,début_tâche&lt;BN$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Semaine d’affichage" prompt="La modification de ce nombre entraînera la défilement du diagramme de Gantt." sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="54" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -4658,7 +5322,67 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D27</xm:sqref>
+          <xm:sqref>D7:D19 D26:D31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{76330665-AA93-4150-A7E6-6D0D1A0B20EF}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D20:D23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7FA9031D-5489-4F15-BD46-DEFB64E198FC}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B21:C21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DF5CD11B-1EFF-4C24-B7C3-2E4277F3C896}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B23:C23</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{85DE7253-C4BE-4E02-B679-A25AB6B6323C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D24:D25</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4681,79 +5405,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B2" s="20"/>
     </row>
     <row r="3" spans="1:2" s="25" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="41" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:2" s="22" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="23" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="19" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="22" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="23" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="75" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="22" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A11" s="23" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="19" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="22" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="23" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4770,23 +5494,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5078,22 +5791,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5120,9 +5840,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>